<commit_message>
add bot con ubicaciones multiples
</commit_message>
<xml_diff>
--- a/Lista de VEPs.xlsx
+++ b/Lista de VEPs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E97952-680D-41BF-93A5-5D045C632404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698B8B25-27FF-48C6-9B3E-2500B9075C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="2" r:id="rId1"/>
@@ -19,17 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista!$A$1:$M$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -404,20 +393,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,7 +431,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Hoja1"/>
@@ -461,9 +446,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -501,9 +486,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,26 +521,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,26 +556,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -783,27 +734,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K2" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -844,1514 +795,1514 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C2" s="4" t="str">
+      <c r="B2" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C2" s="3" t="str">
         <f>VLOOKUP($B2,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D2" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E2" s="4" t="str">
+      <c r="D2" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E2" s="3" t="str">
         <f>VLOOKUP(D2,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F2" s="4" t="str">
+      <c r="F2" s="3" t="str">
         <f>VLOOKUP(B2,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>45047</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="str">
+      <c r="J2" s="3" t="str">
         <f t="shared" ref="J2:J37" si="0">CONCATENATE(TEXT(G2,"MM-YYYY"),"_", TEXT(B2,"00-00000000-0"),"_",H2, "_",E2,".pdf")</f>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="4" t="str">
+      <c r="K2" s="5"/>
+      <c r="L2" s="3" t="str">
         <f>VLOOKUP($B2,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M2" s="4" t="str">
+      <c r="M2" s="3" t="str">
         <f>CONCATENATE(TEXT(G2,"mmyyyy"), " - ",H2, " - ", E2)</f>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C3" s="4" t="str">
+      <c r="B3" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C3" s="3" t="str">
         <f>VLOOKUP($B3,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D3" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E3" s="4" t="str">
+      <c r="D3" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E3" s="3" t="str">
         <f>VLOOKUP(D3,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F3" s="4" t="str">
+      <c r="F3" s="3" t="str">
         <f>VLOOKUP(B3,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>45047</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="str">
+      <c r="J3" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="4" t="str">
+      <c r="K3" s="5"/>
+      <c r="L3" s="3" t="str">
         <f>VLOOKUP($B3,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M3" s="4" t="str">
+      <c r="M3" s="3" t="str">
         <f t="shared" ref="M3:M11" si="1">CONCATENATE(TEXT(G3,"mmyyyy"), " - ",H3, " - ", E3)</f>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C4" s="4" t="str">
+      <c r="B4" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C4" s="3" t="str">
         <f>VLOOKUP($B4,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D4" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E4" s="4" t="str">
+      <c r="D4" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E4" s="3" t="str">
         <f>VLOOKUP(D4,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F4" s="4" t="str">
+      <c r="F4" s="3" t="str">
         <f>VLOOKUP(B4,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>45047</v>
       </c>
       <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="4" t="str">
+      <c r="J4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="4" t="str">
+      <c r="K4" s="5"/>
+      <c r="L4" s="3" t="str">
         <f>VLOOKUP($B4,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M4" s="4" t="str">
+      <c r="M4" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C5" s="4" t="str">
+      <c r="B5" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C5" s="3" t="str">
         <f>VLOOKUP($B5,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D5" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E5" s="4" t="str">
+      <c r="D5" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E5" s="3" t="str">
         <f>VLOOKUP(D5,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F5" s="4" t="str">
+      <c r="F5" s="3" t="str">
         <f>VLOOKUP(B5,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>45047</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="4" t="str">
+      <c r="J5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="4" t="str">
+      <c r="K5" s="5"/>
+      <c r="L5" s="3" t="str">
         <f>VLOOKUP($B5,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M5" s="4" t="str">
+      <c r="M5" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C6" s="4" t="str">
+      <c r="B6" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C6" s="3" t="str">
         <f>VLOOKUP($B6,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D6" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E6" s="4" t="str">
+      <c r="D6" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E6" s="3" t="str">
         <f>VLOOKUP(D6,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F6" s="4" t="str">
+      <c r="F6" s="3" t="str">
         <f>VLOOKUP(B6,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>45047</v>
       </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="4" t="str">
+      <c r="J6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="4" t="str">
+      <c r="K6" s="5"/>
+      <c r="L6" s="3" t="str">
         <f>VLOOKUP($B6,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M6" s="4" t="str">
+      <c r="M6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C7" s="4" t="str">
+      <c r="B7" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C7" s="3" t="str">
         <f>VLOOKUP($B7,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D7" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E7" s="4" t="str">
+      <c r="D7" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E7" s="3" t="str">
         <f>VLOOKUP(D7,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F7" s="4" t="str">
+      <c r="F7" s="3" t="str">
         <f>VLOOKUP(B7,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>45047</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="4" t="str">
+      <c r="J7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="4" t="str">
+      <c r="K7" s="5"/>
+      <c r="L7" s="3" t="str">
         <f>VLOOKUP($B7,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M7" s="4" t="str">
+      <c r="M7" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C8" s="4" t="str">
+      <c r="B8" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C8" s="3" t="str">
         <f>VLOOKUP($B8,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D8" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E8" s="4" t="str">
+      <c r="D8" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E8" s="3" t="str">
         <f>VLOOKUP(D8,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F8" s="4" t="str">
+      <c r="F8" s="3" t="str">
         <f>VLOOKUP(B8,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>45047</v>
       </c>
       <c r="H8" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="4" t="str">
+      <c r="J8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="4" t="str">
+      <c r="K8" s="5"/>
+      <c r="L8" s="3" t="str">
         <f>VLOOKUP($B8,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M8" s="4" t="str">
+      <c r="M8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C9" s="4" t="str">
+      <c r="B9" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C9" s="3" t="str">
         <f>VLOOKUP($B9,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D9" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E9" s="4" t="str">
+      <c r="D9" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E9" s="3" t="str">
         <f>VLOOKUP(D9,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F9" s="4" t="str">
+      <c r="F9" s="3" t="str">
         <f>VLOOKUP(B9,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>44986</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="4" t="str">
+      <c r="J9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>03-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="4" t="str">
+      <c r="K9" s="5"/>
+      <c r="L9" s="3" t="str">
         <f>VLOOKUP($B9,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M9" s="4" t="str">
+      <c r="M9" s="3" t="str">
         <f t="shared" si="1"/>
         <v>032023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C10" s="4" t="str">
+      <c r="B10" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C10" s="3" t="str">
         <f>VLOOKUP($B10,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D10" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E10" s="4" t="str">
+      <c r="D10" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E10" s="3" t="str">
         <f>VLOOKUP(D10,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F10" s="4" t="str">
+      <c r="F10" s="3" t="str">
         <f>VLOOKUP(B10,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>45047</v>
       </c>
       <c r="H10" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="4" t="str">
+      <c r="J10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="4" t="str">
+      <c r="K10" s="5"/>
+      <c r="L10" s="3" t="str">
         <f>VLOOKUP($B10,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M10" s="4" t="str">
+      <c r="M10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C11" s="4" t="str">
+      <c r="B11" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C11" s="3" t="str">
         <f>VLOOKUP($B11,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D11" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E11" s="4" t="str">
+      <c r="D11" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E11" s="3" t="str">
         <f>VLOOKUP(D11,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F11" s="4" t="str">
+      <c r="F11" s="3" t="str">
         <f>VLOOKUP(B11,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>45047</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="4" t="str">
+      <c r="J11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="4" t="str">
+      <c r="K11" s="5"/>
+      <c r="L11" s="3" t="str">
         <f>VLOOKUP($B11,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M11" s="4" t="str">
+      <c r="M11" s="3" t="str">
         <f t="shared" si="1"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C12" s="4" t="str">
+      <c r="B12" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C12" s="3" t="str">
         <f>VLOOKUP($B12,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D12" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E12" s="4" t="str">
+      <c r="D12" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E12" s="3" t="str">
         <f>VLOOKUP(D12,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F12" s="4" t="str">
+      <c r="F12" s="3" t="str">
         <f>VLOOKUP(B12,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>45047</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="4" t="str">
+      <c r="J12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="L12" s="4" t="str">
+      <c r="K12" s="5"/>
+      <c r="L12" s="3" t="str">
         <f>VLOOKUP($B12,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M12" s="4" t="str">
+      <c r="M12" s="3" t="str">
         <f>CONCATENATE(TEXT(G12,"mmyyyy"), " - ",H12, " - ", E12)</f>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C13" s="4" t="str">
+      <c r="B13" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C13" s="3" t="str">
         <f>VLOOKUP($B13,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D13" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E13" s="4" t="str">
+      <c r="D13" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E13" s="3" t="str">
         <f>VLOOKUP(D13,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F13" s="4" t="str">
+      <c r="F13" s="3" t="str">
         <f>VLOOKUP(B13,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>45047</v>
       </c>
       <c r="H13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="4" t="str">
+      <c r="J13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Anticipo Ganancias y Bs Personales _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K13" s="6"/>
-      <c r="L13" s="4" t="str">
+      <c r="K13" s="5"/>
+      <c r="L13" s="3" t="str">
         <f>VLOOKUP($B13,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M13" s="4" t="str">
+      <c r="M13" s="3" t="str">
         <f t="shared" ref="M13:M37" si="2">CONCATENATE(TEXT(G13,"mmyyyy"), " - ",H13, " - ", E13)</f>
         <v>052023 - Anticipo Ganancias y Bs Personales  - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C14" s="4" t="str">
+      <c r="B14" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C14" s="3" t="str">
         <f>VLOOKUP($B14,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D14" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E14" s="4" t="str">
+      <c r="D14" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E14" s="3" t="str">
         <f>VLOOKUP(D14,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F14" s="3" t="str">
         <f>VLOOKUP(B14,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>45047</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="4" t="str">
+      <c r="J14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Anticipo Ganancias y Bs Personales _Juan Perez.pdf</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="4" t="str">
+      <c r="K14" s="5"/>
+      <c r="L14" s="3" t="str">
         <f>VLOOKUP($B14,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M14" s="4" t="str">
+      <c r="M14" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo Ganancias y Bs Personales  - Juan Perez</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C15" s="4" t="str">
+      <c r="B15" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C15" s="3" t="str">
         <f>VLOOKUP($B15,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D15" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E15" s="4" t="str">
+      <c r="D15" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E15" s="3" t="str">
         <f>VLOOKUP(D15,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F15" s="4" t="str">
+      <c r="F15" s="3" t="str">
         <f>VLOOKUP(B15,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>45047</v>
       </c>
       <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="4" t="str">
+      <c r="J15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Anticipo  Bs Personales _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K15" s="6"/>
-      <c r="L15" s="4" t="str">
+      <c r="K15" s="5"/>
+      <c r="L15" s="3" t="str">
         <f>VLOOKUP($B15,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M15" s="4" t="str">
+      <c r="M15" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo  Bs Personales  - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C16" s="4" t="str">
+      <c r="B16" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C16" s="3" t="str">
         <f>VLOOKUP($B16,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D16" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E16" s="4" t="str">
+      <c r="D16" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E16" s="3" t="str">
         <f>VLOOKUP(D16,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F16" s="4" t="str">
+      <c r="F16" s="3" t="str">
         <f>VLOOKUP(B16,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>45047</v>
       </c>
       <c r="H16" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="4" t="str">
+      <c r="J16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Anticipo  Bs Personales _Juan Perez.pdf</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4" t="str">
+      <c r="K16" s="5"/>
+      <c r="L16" s="3" t="str">
         <f>VLOOKUP($B16,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M16" s="4" t="str">
+      <c r="M16" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo  Bs Personales  - Juan Perez</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C17" s="4" t="str">
+      <c r="B17" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C17" s="3" t="str">
         <f>VLOOKUP($B17,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D17" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E17" s="4" t="str">
+      <c r="D17" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E17" s="3" t="str">
         <f>VLOOKUP(D17,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F17" s="4" t="str">
+      <c r="F17" s="3" t="str">
         <f>VLOOKUP(B17,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>45047</v>
       </c>
       <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="4" t="str">
+      <c r="J17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Anticipo  Bs Personales _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="4" t="str">
+      <c r="K17" s="5"/>
+      <c r="L17" s="3" t="str">
         <f>VLOOKUP($B17,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M17" s="4" t="str">
+      <c r="M17" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo  Bs Personales  - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C18" s="4" t="str">
+      <c r="B18" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C18" s="3" t="str">
         <f>VLOOKUP($B18,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D18" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E18" s="4" t="str">
+      <c r="D18" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E18" s="3" t="str">
         <f>VLOOKUP(D18,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F18" s="4" t="str">
+      <c r="F18" s="3" t="str">
         <f>VLOOKUP(B18,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>45047</v>
       </c>
       <c r="H18" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="4" t="str">
+      <c r="J18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Anticipo Ganancias y Bs Personales _Juan Perez.pdf</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4" t="str">
+      <c r="K18" s="5"/>
+      <c r="L18" s="3" t="str">
         <f>VLOOKUP($B18,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M18" s="4" t="str">
+      <c r="M18" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo Ganancias y Bs Personales  - Juan Perez</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C19" s="4" t="str">
+      <c r="B19" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C19" s="3" t="str">
         <f>VLOOKUP($B19,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D19" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E19" s="4" t="str">
+      <c r="D19" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E19" s="3" t="str">
         <f>VLOOKUP(D19,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F19" s="4" t="str">
+      <c r="F19" s="3" t="str">
         <f>VLOOKUP(B19,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>45047</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="4" t="str">
+      <c r="J19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Anticipo  Bs Personales _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="4" t="str">
+      <c r="K19" s="5"/>
+      <c r="L19" s="3" t="str">
         <f>VLOOKUP($B19,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M19" s="4" t="str">
+      <c r="M19" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo  Bs Personales  - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C20" s="4" t="str">
+      <c r="B20" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C20" s="3" t="str">
         <f>VLOOKUP($B20,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D20" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E20" s="4" t="str">
+      <c r="D20" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E20" s="3" t="str">
         <f>VLOOKUP(D20,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F20" s="4" t="str">
+      <c r="F20" s="3" t="str">
         <f>VLOOKUP(B20,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>45047</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="4" t="str">
+      <c r="J20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Anticipo Ganancias y Bs Personales _Juan Perez.pdf</v>
       </c>
-      <c r="K20" s="6"/>
-      <c r="L20" s="4" t="str">
+      <c r="K20" s="5"/>
+      <c r="L20" s="3" t="str">
         <f>VLOOKUP($B20,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M20" s="4" t="str">
+      <c r="M20" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Anticipo Ganancias y Bs Personales  - Juan Perez</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C21" s="4" t="str">
+      <c r="B21" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C21" s="3" t="str">
         <f>VLOOKUP($B21,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D21" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E21" s="4" t="str">
+      <c r="D21" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E21" s="3" t="str">
         <f>VLOOKUP(D21,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F21" s="4" t="str">
+      <c r="F21" s="3" t="str">
         <f>VLOOKUP(B21,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>45047</v>
       </c>
       <c r="H21" t="s">
         <v>9</v>
       </c>
-      <c r="J21" s="4" t="str">
+      <c r="J21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K21" s="6"/>
-      <c r="L21" s="4" t="str">
+      <c r="K21" s="5"/>
+      <c r="L21" s="3" t="str">
         <f>VLOOKUP($B21,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M21" s="4" t="str">
+      <c r="M21" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C22" s="4" t="str">
+      <c r="B22" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C22" s="3" t="str">
         <f>VLOOKUP($B22,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D22" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E22" s="4" t="str">
+      <c r="D22" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E22" s="3" t="str">
         <f>VLOOKUP(D22,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F22" s="4" t="str">
+      <c r="F22" s="3" t="str">
         <f>VLOOKUP(B22,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>45047</v>
       </c>
       <c r="H22" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="4" t="str">
+      <c r="J22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="4" t="str">
+      <c r="K22" s="5"/>
+      <c r="L22" s="3" t="str">
         <f>VLOOKUP($B22,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M22" s="4" t="str">
+      <c r="M22" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C23" s="4" t="str">
+      <c r="B23" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C23" s="3" t="str">
         <f>VLOOKUP($B23,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D23" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E23" s="4" t="str">
+      <c r="D23" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E23" s="3" t="str">
         <f>VLOOKUP(D23,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F23" s="4" t="str">
+      <c r="F23" s="3" t="str">
         <f>VLOOKUP(B23,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>45047</v>
       </c>
       <c r="H23" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="4" t="str">
+      <c r="J23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="4" t="str">
+      <c r="K23" s="5"/>
+      <c r="L23" s="3" t="str">
         <f>VLOOKUP($B23,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M23" s="4" t="str">
+      <c r="M23" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C24" s="4" t="str">
+      <c r="B24" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C24" s="3" t="str">
         <f>VLOOKUP($B24,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D24" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E24" s="4" t="str">
+      <c r="D24" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E24" s="3" t="str">
         <f>VLOOKUP(D24,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F24" s="4" t="str">
+      <c r="F24" s="3" t="str">
         <f>VLOOKUP(B24,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>45047</v>
       </c>
       <c r="H24" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="4" t="str">
+      <c r="J24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K24" s="6"/>
-      <c r="L24" s="4" t="str">
+      <c r="K24" s="5"/>
+      <c r="L24" s="3" t="str">
         <f>VLOOKUP($B24,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M24" s="4" t="str">
+      <c r="M24" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C25" s="4" t="str">
+      <c r="B25" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C25" s="3" t="str">
         <f>VLOOKUP($B25,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D25" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E25" s="4" t="str">
+      <c r="D25" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E25" s="3" t="str">
         <f>VLOOKUP(D25,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F25" s="4" t="str">
+      <c r="F25" s="3" t="str">
         <f>VLOOKUP(B25,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>45047</v>
       </c>
       <c r="H25" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="4" t="str">
+      <c r="J25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="4" t="str">
+      <c r="K25" s="5"/>
+      <c r="L25" s="3" t="str">
         <f>VLOOKUP($B25,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M25" s="4" t="str">
+      <c r="M25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C26" s="4" t="str">
+      <c r="B26" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C26" s="3" t="str">
         <f>VLOOKUP($B26,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D26" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E26" s="4" t="str">
+      <c r="D26" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E26" s="3" t="str">
         <f>VLOOKUP(D26,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F26" s="4" t="str">
+      <c r="F26" s="3" t="str">
         <f>VLOOKUP(B26,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>45047</v>
       </c>
       <c r="H26" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="4" t="str">
+      <c r="J26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="4" t="str">
+      <c r="K26" s="5"/>
+      <c r="L26" s="3" t="str">
         <f>VLOOKUP($B26,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M26" s="4" t="str">
+      <c r="M26" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C27" s="4" t="str">
+      <c r="B27" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C27" s="3" t="str">
         <f>VLOOKUP($B27,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D27" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E27" s="4" t="str">
+      <c r="D27" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E27" s="3" t="str">
         <f>VLOOKUP(D27,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F27" s="4" t="str">
+      <c r="F27" s="3" t="str">
         <f>VLOOKUP(B27,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>45047</v>
       </c>
       <c r="H27" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="4" t="str">
+      <c r="J27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K27" s="6"/>
-      <c r="L27" s="4" t="str">
+      <c r="K27" s="5"/>
+      <c r="L27" s="3" t="str">
         <f>VLOOKUP($B27,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M27" s="4" t="str">
+      <c r="M27" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
-      <c r="B28" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C28" s="4" t="str">
+      <c r="B28" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C28" s="3" t="str">
         <f>VLOOKUP($B28,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D28" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E28" s="4" t="str">
+      <c r="D28" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E28" s="3" t="str">
         <f>VLOOKUP(D28,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F28" s="4" t="str">
+      <c r="F28" s="3" t="str">
         <f>VLOOKUP(B28,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>45047</v>
       </c>
       <c r="H28" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="4" t="str">
+      <c r="J28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K28" s="6"/>
-      <c r="L28" s="4" t="str">
+      <c r="K28" s="5"/>
+      <c r="L28" s="3" t="str">
         <f>VLOOKUP($B28,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M28" s="4" t="str">
+      <c r="M28" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>30</v>
       </c>
-      <c r="B29" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C29" s="4" t="str">
+      <c r="B29" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C29" s="3" t="str">
         <f>VLOOKUP($B29,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D29" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E29" s="4" t="str">
+      <c r="D29" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E29" s="3" t="str">
         <f>VLOOKUP(D29,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F29" s="4" t="str">
+      <c r="F29" s="3" t="str">
         <f>VLOOKUP(B29,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>45047</v>
       </c>
       <c r="H29" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="4" t="str">
+      <c r="J29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K29" s="6"/>
-      <c r="L29" s="4" t="str">
+      <c r="K29" s="5"/>
+      <c r="L29" s="3" t="str">
         <f>VLOOKUP($B29,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M29" s="4" t="str">
+      <c r="M29" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>31</v>
       </c>
-      <c r="B30" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C30" s="4" t="str">
+      <c r="B30" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C30" s="3" t="str">
         <f>VLOOKUP($B30,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D30" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E30" s="4" t="str">
+      <c r="D30" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E30" s="3" t="str">
         <f>VLOOKUP(D30,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F30" s="4" t="str">
+      <c r="F30" s="3" t="str">
         <f>VLOOKUP(B30,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>45047</v>
       </c>
       <c r="H30" t="s">
         <v>9</v>
       </c>
-      <c r="J30" s="4" t="str">
+      <c r="J30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="4" t="str">
+      <c r="K30" s="5"/>
+      <c r="L30" s="3" t="str">
         <f>VLOOKUP($B30,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M30" s="4" t="str">
+      <c r="M30" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>32</v>
       </c>
-      <c r="B31" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C31" s="4" t="str">
+      <c r="B31" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C31" s="3" t="str">
         <f>VLOOKUP($B31,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D31" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E31" s="4" t="str">
+      <c r="D31" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E31" s="3" t="str">
         <f>VLOOKUP(D31,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F31" s="4" t="str">
+      <c r="F31" s="3" t="str">
         <f>VLOOKUP(B31,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <v>45047</v>
       </c>
       <c r="H31" t="s">
         <v>9</v>
       </c>
-      <c r="J31" s="4" t="str">
+      <c r="J31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K31" s="6"/>
-      <c r="L31" s="4" t="str">
+      <c r="K31" s="5"/>
+      <c r="L31" s="3" t="str">
         <f>VLOOKUP($B31,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M31" s="4" t="str">
+      <c r="M31" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>33</v>
       </c>
-      <c r="B32" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C32" s="4" t="str">
+      <c r="B32" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C32" s="3" t="str">
         <f>VLOOKUP($B32,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D32" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E32" s="4" t="str">
+      <c r="D32" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E32" s="3" t="str">
         <f>VLOOKUP(D32,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="F32" s="3" t="str">
         <f>VLOOKUP(B32,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>45047</v>
       </c>
       <c r="H32" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="4" t="str">
+      <c r="J32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="4" t="str">
+      <c r="K32" s="5"/>
+      <c r="L32" s="3" t="str">
         <f>VLOOKUP($B32,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M32" s="4" t="str">
+      <c r="M32" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>34</v>
       </c>
-      <c r="B33" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C33" s="4" t="str">
+      <c r="B33" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C33" s="3" t="str">
         <f>VLOOKUP($B33,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D33" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E33" s="4" t="str">
+      <c r="D33" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E33" s="3" t="str">
         <f>VLOOKUP(D33,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F33" s="4" t="str">
+      <c r="F33" s="3" t="str">
         <f>VLOOKUP(B33,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <v>45047</v>
       </c>
       <c r="H33" t="s">
         <v>9</v>
       </c>
-      <c r="J33" s="4" t="str">
+      <c r="J33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Autonomos_Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="4" t="str">
+      <c r="K33" s="5"/>
+      <c r="L33" s="3" t="str">
         <f>VLOOKUP($B33,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M33" s="4" t="str">
+      <c r="M33" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>35</v>
       </c>
-      <c r="B34" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C34" s="4" t="str">
+      <c r="B34" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C34" s="3" t="str">
         <f>VLOOKUP($B34,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D34" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E34" s="4" t="str">
+      <c r="D34" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E34" s="3" t="str">
         <f>VLOOKUP(D34,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F34" s="4" t="str">
+      <c r="F34" s="3" t="str">
         <f>VLOOKUP(B34,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <v>45047</v>
       </c>
       <c r="H34" t="s">
         <v>9</v>
       </c>
-      <c r="J34" s="4" t="str">
+      <c r="J34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Autonomos_Juan Perez.pdf</v>
       </c>
-      <c r="K34" s="6"/>
-      <c r="L34" s="4" t="str">
+      <c r="K34" s="5"/>
+      <c r="L34" s="3" t="str">
         <f>VLOOKUP($B34,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M34" s="4" t="str">
+      <c r="M34" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Autonomos - Juan Perez</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36</v>
       </c>
-      <c r="B35" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C35" s="4" t="str">
+      <c r="B35" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C35" s="3" t="str">
         <f>VLOOKUP($B35,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D35" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E35" s="4" t="str">
+      <c r="D35" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E35" s="3" t="str">
         <f>VLOOKUP(D35,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F35" s="4" t="str">
+      <c r="F35" s="3" t="str">
         <f>VLOOKUP(B35,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <v>45047</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="4" t="str">
+      <c r="J35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Monotributo _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K35" s="6"/>
-      <c r="L35" s="4" t="str">
+      <c r="K35" s="5"/>
+      <c r="L35" s="3" t="str">
         <f>VLOOKUP($B35,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M35" s="4" t="str">
+      <c r="M35" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Monotributo  - Gian Franco Lorenzo Patti</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>37</v>
       </c>
-      <c r="B36" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="C36" s="4" t="str">
+      <c r="B36" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="C36" s="3" t="str">
         <f>VLOOKUP($B36,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>clavefalsa123</v>
       </c>
-      <c r="D36" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="E36" s="4" t="str">
+      <c r="D36" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="E36" s="3" t="str">
         <f>VLOOKUP(D36,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Juan Perez</v>
       </c>
-      <c r="F36" s="4" t="str">
+      <c r="F36" s="3" t="str">
         <f>VLOOKUP(B36,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Red Link</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <v>45047</v>
       </c>
       <c r="H36" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="4" t="str">
+      <c r="J36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_27-00000000-6_Monotributo _Juan Perez.pdf</v>
       </c>
-      <c r="K36" s="6"/>
-      <c r="L36" s="4" t="str">
+      <c r="K36" s="5"/>
+      <c r="L36" s="3" t="str">
         <f>VLOOKUP($B36,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M36" s="4" t="str">
+      <c r="M36" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Monotributo  - Juan Perez</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>38</v>
       </c>
-      <c r="B37" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="C37" s="4" t="str">
+      <c r="B37" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="C37" s="3" t="str">
         <f>VLOOKUP($B37,Contribuyentes!$A$2:$F$29,2,FALSE)</f>
         <v>claveprueba123</v>
       </c>
-      <c r="D37" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="E37" s="4" t="str">
+      <c r="D37" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="E37" s="3" t="str">
         <f>VLOOKUP(D37,Contribuyentes!$A$2:$F$29,5,FALSE)</f>
         <v>Gian Franco Lorenzo Patti</v>
       </c>
-      <c r="F37" s="4" t="str">
+      <c r="F37" s="3" t="str">
         <f>VLOOKUP(B37,Contribuyentes!$A$2:$F$29,6,FALSE)</f>
         <v>Pago Mis Cuentas</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>45047</v>
       </c>
       <c r="H37" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="4" t="str">
+      <c r="J37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>05-2023_23-00000000-6_Monotributo _Gian Franco Lorenzo Patti.pdf</v>
       </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="4" t="str">
+      <c r="K37" s="5"/>
+      <c r="L37" s="3" t="str">
         <f>VLOOKUP($B37,Contribuyentes!$A$2:$G$29,7,FALSE)</f>
         <v>mail@gmail.com.ar</v>
       </c>
-      <c r="M37" s="4" t="str">
+      <c r="M37" s="3" t="str">
         <f t="shared" si="2"/>
         <v>052023 - Monotributo  - Gian Franco Lorenzo Patti</v>
       </c>
@@ -2372,449 +2323,446 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>27000000006</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>27000000006</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="17" t="e">
+      <c r="C2" s="13" t="e">
         <f>VLOOKUP(A2,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D2" s="17" t="e">
+      <c r="D2" s="13" t="e">
         <f>IF(EXACT(B2,C2),"OK","MAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>23000000006</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>23000000006</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="17" t="e">
+      <c r="C3" s="13" t="e">
         <f>VLOOKUP(A3,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D3" s="17" t="e">
+      <c r="D3" s="13" t="e">
         <f t="shared" ref="D3:D29" si="0">IF(EXACT(B3,C3),"OK","MAL")</f>
         <v>#REF!</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="17" t="e">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="13" t="e">
         <f>VLOOKUP(A4,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D4" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="17" t="e">
+      <c r="D4" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="13" t="e">
         <f>VLOOKUP(A5,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D5" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="17" t="e">
+      <c r="D5" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="13" t="e">
         <f>VLOOKUP(A6,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="17" t="e">
+      <c r="D6" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="13" t="e">
         <f>VLOOKUP(A7,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D7" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="17" t="e">
+      <c r="D7" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="13" t="e">
         <f>VLOOKUP(A8,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D8" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="17" t="e">
+      <c r="D8" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="13" t="e">
         <f>VLOOKUP(A9,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D9" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="17" t="e">
+      <c r="D9" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="13" t="e">
         <f>VLOOKUP(A10,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D10" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="17" t="e">
+      <c r="D10" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="13" t="e">
         <f>VLOOKUP(A11,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="17" t="e">
+      <c r="D11" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="13" t="e">
         <f>VLOOKUP(A12,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D12" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="17" t="e">
+      <c r="D12" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="13" t="e">
         <f>VLOOKUP(A13,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D13" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="e">
+      <c r="D13" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="13" t="e">
         <f>VLOOKUP(A14,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D14" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="17" t="e">
+      <c r="D14" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="13" t="e">
         <f>VLOOKUP(A15,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D15" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="17" t="e">
+      <c r="D15" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C16" s="13" t="e">
         <f>VLOOKUP(A16,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D16" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="17" t="e">
+      <c r="D16" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="13" t="e">
         <f>VLOOKUP(A17,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D17" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E17"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="17" t="e">
+      <c r="D17" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="13" t="e">
         <f>VLOOKUP(A18,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D18" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="17" t="e">
+      <c r="D18" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="13" t="e">
         <f>VLOOKUP(A19,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D19" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E19" s="14"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="17" t="e">
+      <c r="D19" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="13" t="e">
         <f>VLOOKUP(A20,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D20" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="17" t="e">
+      <c r="D20" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="13" t="e">
         <f>VLOOKUP(A21,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D21" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="17" t="e">
+      <c r="D21" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="13" t="e">
         <f>VLOOKUP(A22,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D22" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="17" t="e">
+      <c r="D22" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="13" t="e">
         <f>VLOOKUP(A23,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D23" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="17" t="e">
+      <c r="D23" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="13" t="e">
         <f>VLOOKUP(A24,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D24" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E24" s="14"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="17" t="e">
+      <c r="D24" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="13" t="e">
         <f>VLOOKUP(A25,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D25" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E25" s="14"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="17" t="e">
+      <c r="D25" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="13" t="e">
         <f>VLOOKUP(A26,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D26" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="17" t="e">
+      <c r="D26" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="13" t="e">
         <f>VLOOKUP(A27,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D27" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E27" s="14"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="17" t="e">
+      <c r="D27" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="13" t="e">
         <f>VLOOKUP(A28,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D28" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="17" t="e">
+      <c r="D28" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="13" t="e">
         <f>VLOOKUP(A29,[1]!Tabla1[[CUIT SOCIO]:[clave afip]],2,FALSE)</f>
         <v>#REF!</v>
       </c>
-      <c r="D29" s="17" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="E29" s="14"/>
-      <c r="G29" s="9"/>
+      <c r="D29" s="13" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="G29" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>

</xml_diff>